<commit_message>
Fixed many issues, improved and fixed many tests
</commit_message>
<xml_diff>
--- a/XlsEpplus.Test/testfiles/datatype-checks.xlsx
+++ b/XlsEpplus.Test/testfiles/datatype-checks.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Boolean</t>
   </si>
@@ -22,12 +22,6 @@
     <t>01.01.1600</t>
   </si>
   <si>
-    <t>Datetime2mindate</t>
-  </si>
-  <si>
-    <t>Datetime4macmindate</t>
-  </si>
-  <si>
     <t>Datetime 3 too early date</t>
   </si>
   <si>
@@ -77,12 +71,48 @@
   </si>
   <si>
     <t>Time2a</t>
+  </si>
+  <si>
+    <t>Byte</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Char</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Time1a</t>
+  </si>
+  <si>
+    <t>Datetime2MaxDate</t>
+  </si>
+  <si>
+    <t>Datetime2MinDate</t>
+  </si>
+  <si>
+    <t>Datetime4MacMinDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,13 +142,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -137,7 +168,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -423,73 +454,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="15" customWidth="1"/>
-    <col min="17" max="18" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="7" width="15" customWidth="1"/>
+    <col min="19" max="20" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
+      <c r="W1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -502,56 +563,84 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="1">
+        <v>2958465</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>1828.6354166666667</v>
       </c>
-      <c r="G2" t="e">
+      <c r="H2" t="e">
         <f>8/0</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H2" t="e">
+      <c r="I2" t="e">
         <f>a0</f>
         <v>#NAME?</v>
       </c>
-      <c r="I2" t="e">
+      <c r="J2" t="e">
         <f>INT("kjk")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J2" t="e">
+      <c r="K2" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="K2">
+      <c r="L2">
+        <f ca="1">M2</f>
+        <v>0</v>
+      </c>
+      <c r="M2">
         <f ca="1">L2</f>
         <v>0</v>
       </c>
-      <c r="L2">
-        <f ca="1">K2</f>
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>14</v>
+      <c r="N2" t="s">
+        <v>12</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" s="3">
+        <v>12</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="3">
         <v>0.63541666666666663</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="R2" s="6">
+        <v>0.64969907407407412</v>
+      </c>
+      <c r="S2" s="4">
         <v>10.684259259259258</v>
       </c>
-      <c r="R2" s="5">
+      <c r="T2" s="5">
         <v>10.684259259259258</v>
+      </c>
+      <c r="U2">
+        <v>2</v>
+      </c>
+      <c r="V2">
+        <v>1.4532499999999999</v>
+      </c>
+      <c r="W2" t="s">
+        <v>25</v>
+      </c>
+      <c r="X2">
+        <v>39211212.3434733</v>
+      </c>
+      <c r="Y2">
+        <v>289382</v>
+      </c>
+      <c r="Z2">
+        <v>2297987128</v>
+      </c>
+      <c r="AA2">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>